<commit_message>
Updating visual classification distribution and distribution of bars in disk galaxies
</commit_message>
<xml_diff>
--- a/results/morphology/visual_classification_LC.xlsx
+++ b/results/morphology/visual_classification_LC.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/costantin/Documents/TEACHING/Thesis/Master/2023/Leonor_Arriscado_Nunes/Visual_classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FF5FB5A-E276-E24B-928D-529D6DD3B9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{012C474D-1357-D544-9B16-88D779FB9495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -142,7 +155,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -444,21 +457,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="167" zoomScaleNormal="167" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="5"/>
-    <col min="2" max="2" width="21.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17" style="7" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="5"/>
+    <col min="1" max="1" width="8.875" style="5"/>
+    <col min="2" max="2" width="21.7890625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.0078125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.94921875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.94921875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="42.375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="24.2109375" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2585,10 +2598,10 @@
         <v>0</v>
       </c>
       <c r="C93" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93" s="6">
         <v>0</v>

</xml_diff>